<commit_message>
Reviewed Scrum backlog and Spring Planing for first sprint.
</commit_message>
<xml_diff>
--- a/Documents/Task 10/scrum_v02.xlsx
+++ b/Documents/Task 10/scrum_v02.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="120" windowWidth="16488" windowHeight="9312" activeTab="1"/>
+    <workbookView xWindow="384" yWindow="120" windowWidth="16488" windowHeight="9312" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="68">
   <si>
     <t>ID</t>
   </si>
@@ -34,27 +34,9 @@
     <t>Status</t>
   </si>
   <si>
-    <t>high</t>
-  </si>
-  <si>
-    <t>medium</t>
-  </si>
-  <si>
-    <t>low</t>
-  </si>
-  <si>
-    <t>waiting</t>
-  </si>
-  <si>
     <t>work in progress</t>
   </si>
   <si>
-    <t>done</t>
-  </si>
-  <si>
-    <t>cancelled</t>
-  </si>
-  <si>
     <t>Owner</t>
   </si>
   <si>
@@ -70,36 +52,9 @@
     <t>Effort Actual</t>
   </si>
   <si>
-    <t>Martin</t>
-  </si>
-  <si>
-    <t>Hans</t>
-  </si>
-  <si>
-    <t>Tom</t>
-  </si>
-  <si>
-    <t>Jennifer</t>
-  </si>
-  <si>
-    <t>Database</t>
-  </si>
-  <si>
     <t>UI, Controller</t>
   </si>
   <si>
-    <t>All</t>
-  </si>
-  <si>
-    <t>Main Window</t>
-  </si>
-  <si>
-    <t>Patient Model</t>
-  </si>
-  <si>
-    <t>Data model for patient record needs to be created based on standard....</t>
-  </si>
-  <si>
     <t>Effort Plan Original</t>
   </si>
   <si>
@@ -224,6 +179,48 @@
   </si>
   <si>
     <t>Anna tracks her medication changes.</t>
+  </si>
+  <si>
+    <t>Medication Data Model</t>
+  </si>
+  <si>
+    <t>Database, JPA Classes</t>
+  </si>
+  <si>
+    <t>Navigation</t>
+  </si>
+  <si>
+    <t>Medication overview</t>
+  </si>
+  <si>
+    <t>UI, Controller, Modell</t>
+  </si>
+  <si>
+    <t>Implement the Design as planned</t>
+  </si>
+  <si>
+    <t>Data model for medication records needs to be created based on our developed class diagram. Create some simple example data</t>
+  </si>
+  <si>
+    <t>Create top Navigation and View Controller, which can be used on every page</t>
+  </si>
+  <si>
+    <t>Marwin</t>
+  </si>
+  <si>
+    <t>Mete</t>
+  </si>
+  <si>
+    <t>Amin</t>
+  </si>
+  <si>
+    <t>Carole</t>
+  </si>
+  <si>
+    <t>Michel</t>
+  </si>
+  <si>
+    <t>Jonas</t>
   </si>
 </sst>
 </file>
@@ -657,55 +654,55 @@
         <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -717,8 +714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -738,7 +735,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
@@ -747,97 +744,98 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E2" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3"/>
+      <c r="E3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E4">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>5</v>
-      </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="E5">
-        <v>40</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="E6">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="E7">
         <v>20</v>
@@ -845,41 +843,41 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="E8">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="E9">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="E10">
         <v>10</v>
@@ -887,30 +885,31 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="E11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
-        <v>57</v>
-      </c>
-      <c r="C12" t="s">
-        <v>68</v>
-      </c>
-      <c r="E12">
-        <v>30</v>
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -924,19 +923,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.77734375" customWidth="1"/>
     <col min="2" max="2" width="6.21875" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="19.44140625" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" customWidth="1"/>
+    <col min="3" max="3" width="20.21875" customWidth="1"/>
+    <col min="4" max="4" width="66.6640625" customWidth="1"/>
+    <col min="5" max="5" width="18.77734375" customWidth="1"/>
     <col min="6" max="6" width="10.33203125" customWidth="1"/>
     <col min="7" max="7" width="9.77734375" customWidth="1"/>
     <col min="8" max="8" width="8.33203125" customWidth="1"/>
@@ -951,7 +950,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>1</v>
@@ -960,66 +959,60 @@
         <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1.1000000000000001</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>62</v>
       </c>
       <c r="G2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" t="s">
-        <v>6</v>
+        <v>63</v>
       </c>
       <c r="I2">
-        <v>2</v>
-      </c>
-      <c r="J2">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
       <c r="L2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -1027,31 +1020,31 @@
         <v>1.2</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" t="s">
+        <v>61</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>66</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" t="s">
+        <v>67</v>
+      </c>
+      <c r="I3">
+        <v>12</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3" t="s">
         <v>5</v>
-      </c>
-      <c r="I3">
-        <v>8</v>
-      </c>
-      <c r="J3">
-        <v>6</v>
-      </c>
-      <c r="K3">
-        <v>4</v>
-      </c>
-      <c r="L3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -1061,94 +1054,29 @@
       <c r="B4">
         <v>1</v>
       </c>
+      <c r="C4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" t="s">
+        <v>59</v>
+      </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="G4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I4">
+        <v>12</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4" t="s">
         <v>5</v>
-      </c>
-      <c r="I4">
-        <v>16</v>
-      </c>
-      <c r="J4">
-        <v>20</v>
-      </c>
-      <c r="K4">
-        <f>SUM(J4:J4)</f>
-        <v>20</v>
-      </c>
-      <c r="L4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>2.1</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5">
-        <v>4</v>
-      </c>
-      <c r="J5">
-        <v>10</v>
-      </c>
-      <c r="K5">
-        <v>4</v>
-      </c>
-      <c r="L5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="E6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" t="s">
-        <v>5</v>
-      </c>
-      <c r="I6">
-        <v>8</v>
-      </c>
-      <c r="J6">
-        <v>6</v>
-      </c>
-      <c r="K6">
-        <v>5</v>
-      </c>
-      <c r="L6" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1173,16 +1101,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="5" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Removed Mapping-Errors due to Typos, Java Version 8 in POM, updated the scrum Backlog.
</commit_message>
<xml_diff>
--- a/Documents/Task 10/scrum_v02.xlsx
+++ b/Documents/Task 10/scrum_v02.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="120" windowWidth="16488" windowHeight="9312" activeTab="2"/>
+    <workbookView xWindow="384" yWindow="120" windowWidth="16488" windowHeight="7812" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="85">
   <si>
     <t>ID</t>
   </si>
@@ -221,6 +221,58 @@
   </si>
   <si>
     <t>Jonas</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>Medication entry View</t>
+  </si>
+  <si>
+    <t>Create the planned Views for the entry of a new Medicament</t>
+  </si>
+  <si>
+    <t>Optimize the medication dose schema to enter a new Medicament</t>
+  </si>
+  <si>
+    <t>Modell, Database</t>
+  </si>
+  <si>
+    <t>Validate and save an entered medicament</t>
+  </si>
+  <si>
+    <t>Navigate to the new View and Back</t>
+  </si>
+  <si>
+    <t>Controller, Modell</t>
+  </si>
+  <si>
+    <t>Medication validation</t>
+  </si>
+  <si>
+    <t>Navigate to the new view over the Medicationoverview-List</t>
+  </si>
+  <si>
+    <t>Medication edit View</t>
+  </si>
+  <si>
+    <t>Create the planned Editing view to edit an existing medicament by using 2,3.
+Do not implement history yet.</t>
+  </si>
+  <si>
+    <t>Stop a Medication</t>
+  </si>
+  <si>
+    <t>Stop an existing Medication over the Medicationoverview-List</t>
+  </si>
+  <si>
+    <t>GUI Optimization</t>
+  </si>
+  <si>
+    <t>UI</t>
+  </si>
+  <si>
+    <t>Create a nice SCSS file to beautify our GUI</t>
   </si>
 </sst>
 </file>
@@ -276,7 +328,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -294,6 +346,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -715,14 +770,14 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B3" sqref="B3:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.6640625" customWidth="1"/>
     <col min="2" max="2" width="33.5546875" customWidth="1"/>
-    <col min="3" max="3" width="31.21875" customWidth="1"/>
+    <col min="3" max="3" width="38.44140625" customWidth="1"/>
     <col min="4" max="4" width="9.44140625" customWidth="1"/>
     <col min="5" max="5" width="18.6640625" customWidth="1"/>
     <col min="6" max="6" width="19.5546875" customWidth="1"/>
@@ -923,10 +978,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -934,7 +989,7 @@
     <col min="1" max="1" width="4.77734375" customWidth="1"/>
     <col min="2" max="2" width="6.21875" customWidth="1"/>
     <col min="3" max="3" width="20.21875" customWidth="1"/>
-    <col min="4" max="4" width="66.6640625" customWidth="1"/>
+    <col min="4" max="4" width="85.44140625" customWidth="1"/>
     <col min="5" max="5" width="18.77734375" customWidth="1"/>
     <col min="6" max="6" width="10.33203125" customWidth="1"/>
     <col min="7" max="7" width="9.77734375" customWidth="1"/>
@@ -1009,10 +1064,10 @@
         <v>12</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="L2" t="s">
-        <v>5</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -1041,10 +1096,10 @@
         <v>12</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="L3" t="s">
-        <v>5</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -1073,9 +1128,241 @@
         <v>12</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="L4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2.1</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" t="s">
+        <v>64</v>
+      </c>
+      <c r="I5">
+        <v>20</v>
+      </c>
+      <c r="L5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G6" t="s">
+        <v>66</v>
+      </c>
+      <c r="I6">
+        <v>10</v>
+      </c>
+      <c r="L6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7" t="s">
+        <v>67</v>
+      </c>
+      <c r="G7" t="s">
+        <v>62</v>
+      </c>
+      <c r="I7">
+        <v>15</v>
+      </c>
+      <c r="L7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>2.4</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>65</v>
+      </c>
+      <c r="G8" t="s">
+        <v>67</v>
+      </c>
+      <c r="I8">
+        <v>4</v>
+      </c>
+      <c r="L8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>3.1</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9" t="s">
+        <v>63</v>
+      </c>
+      <c r="I9">
+        <v>10</v>
+      </c>
+      <c r="L9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>3.2</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" t="s">
+        <v>65</v>
+      </c>
+      <c r="G10" t="s">
+        <v>67</v>
+      </c>
+      <c r="I10">
+        <v>5</v>
+      </c>
+      <c r="L10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" t="s">
+        <v>81</v>
+      </c>
+      <c r="E11" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" t="s">
+        <v>66</v>
+      </c>
+      <c r="G11" t="s">
+        <v>62</v>
+      </c>
+      <c r="I11">
+        <v>10</v>
+      </c>
+      <c r="L11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>1.4</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12" t="s">
+        <v>83</v>
+      </c>
+      <c r="F12" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" t="s">
+        <v>64</v>
+      </c>
+      <c r="I12">
+        <v>10</v>
+      </c>
+      <c r="L12" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
preplaning of sprint 3
</commit_message>
<xml_diff>
--- a/Documents/Task 10/scrum_v02.xlsx
+++ b/Documents/Task 10/scrum_v02.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michel\workspace\ch.bfh.btx8081.w2015.schwarz\Documents\Task 10\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Turna\workspace\ch.bfh.btx8081.w2015.schwarz\trunk\Documents\Task 10\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="384" yWindow="120" windowWidth="16488" windowHeight="7812" activeTab="3"/>
+    <workbookView xWindow="390" yWindow="120" windowWidth="16485" windowHeight="7815" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
@@ -17,12 +17,12 @@
     <sheet name="Sprint Backlog" sheetId="2" r:id="rId3"/>
     <sheet name="BurndownChart" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="119">
   <si>
     <t>ID</t>
   </si>
@@ -335,12 +335,57 @@
   </si>
   <si>
     <t>Sprint3</t>
+  </si>
+  <si>
+    <t>Unit Test's</t>
+  </si>
+  <si>
+    <t>Medication Photo</t>
+  </si>
+  <si>
+    <t>Create for the logical classes unit test's for testing</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Implement the photo of the medication</t>
+  </si>
+  <si>
+    <t>Prescription historization</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">historization the Insert, editing, and deleting of the Prescription </t>
+  </si>
+  <si>
+    <t>Medication extern Information</t>
+  </si>
+  <si>
+    <t>Insert a Compendium link for additional information</t>
+  </si>
+  <si>
+    <t>Alert Popup</t>
+  </si>
+  <si>
+    <t>Create a login page for the patient</t>
+  </si>
+  <si>
+    <t>not used</t>
+  </si>
+  <si>
+    <t>sprint 3</t>
+  </si>
+  <si>
+    <t>Create a alert popup for the daily medication with applied funktion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -509,6 +554,9 @@
       <alignment textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -524,9 +572,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -570,7 +615,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
@@ -664,6 +709,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0578-4E58-90C1-91993B39FDE3}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -746,6 +796,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0578-4E58-90C1-91993B39FDE3}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="0"/>
@@ -811,6 +866,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-0578-4E58-90C1-91993B39FDE3}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -855,7 +915,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -970,7 +1029,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1039,7 +1097,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1665,7 +1722,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1957,13 +2014,13 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="3" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1971,7 +2028,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1979,7 +2036,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1987,7 +2044,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1995,7 +2052,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -2003,7 +2060,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -2011,7 +2068,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -2029,22 +2086,22 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E12"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" customWidth="1"/>
-    <col min="2" max="2" width="33.5546875" customWidth="1"/>
-    <col min="3" max="3" width="38.44140625" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" customWidth="1"/>
-    <col min="6" max="6" width="19.5546875" customWidth="1"/>
-    <col min="7" max="7" width="13.44140625" customWidth="1"/>
-    <col min="8" max="8" width="14.44140625" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="33.5703125" customWidth="1"/>
+    <col min="3" max="3" width="38.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2070,7 +2127,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2083,8 +2140,11 @@
       <c r="E2">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2098,8 +2158,11 @@
       <c r="E3">
         <v>50</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H3" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2112,8 +2175,11 @@
       <c r="E4">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2126,8 +2192,11 @@
       <c r="E5">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2140,8 +2209,11 @@
       <c r="E6">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2154,8 +2226,11 @@
       <c r="E7">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2168,8 +2243,11 @@
       <c r="E8">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2182,8 +2260,11 @@
       <c r="E9">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2196,8 +2277,11 @@
       <c r="E10">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2210,8 +2294,11 @@
       <c r="E11">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -2224,6 +2311,9 @@
       <c r="D12" s="1"/>
       <c r="E12" s="1">
         <v>20</v>
+      </c>
+      <c r="H12" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -2237,29 +2327,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.77734375" customWidth="1"/>
-    <col min="2" max="2" width="6.21875" customWidth="1"/>
-    <col min="3" max="3" width="20.21875" customWidth="1"/>
-    <col min="4" max="4" width="85.44140625" customWidth="1"/>
-    <col min="5" max="5" width="18.77734375" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" customWidth="1"/>
-    <col min="7" max="7" width="9.77734375" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" customWidth="1"/>
-    <col min="9" max="9" width="7.88671875" customWidth="1"/>
-    <col min="10" max="10" width="9.109375" customWidth="1"/>
-    <col min="11" max="11" width="7.21875" customWidth="1"/>
-    <col min="12" max="12" width="15.21875" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" customWidth="1"/>
+    <col min="4" max="4" width="85.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" customWidth="1"/>
+    <col min="11" max="11" width="7.28515625" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="4" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2297,7 +2387,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1.1000000000000001</v>
       </c>
@@ -2329,7 +2419,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1.2</v>
       </c>
@@ -2361,7 +2451,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1.3</v>
       </c>
@@ -2393,7 +2483,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2.1</v>
       </c>
@@ -2419,10 +2509,10 @@
         <v>20</v>
       </c>
       <c r="L5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2.2000000000000002</v>
       </c>
@@ -2447,11 +2537,14 @@
       <c r="I6">
         <v>10</v>
       </c>
+      <c r="K6">
+        <v>5</v>
+      </c>
       <c r="L6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2.2999999999999998</v>
       </c>
@@ -2477,10 +2570,10 @@
         <v>15</v>
       </c>
       <c r="L7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2.4</v>
       </c>
@@ -2506,10 +2599,10 @@
         <v>4</v>
       </c>
       <c r="L8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3.1</v>
       </c>
@@ -2535,10 +2628,10 @@
         <v>10</v>
       </c>
       <c r="L9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3.2</v>
       </c>
@@ -2564,10 +2657,10 @@
         <v>5</v>
       </c>
       <c r="L10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4.0999999999999996</v>
       </c>
@@ -2593,10 +2686,10 @@
         <v>10</v>
       </c>
       <c r="L11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1.4</v>
       </c>
@@ -2622,6 +2715,144 @@
         <v>10</v>
       </c>
       <c r="L12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>104</v>
+      </c>
+      <c r="D13" t="s">
+        <v>106</v>
+      </c>
+      <c r="E13" t="s">
+        <v>107</v>
+      </c>
+      <c r="I13">
+        <v>10</v>
+      </c>
+      <c r="L13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1.5</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D14" t="s">
+        <v>108</v>
+      </c>
+      <c r="E14" t="s">
+        <v>79</v>
+      </c>
+      <c r="I14">
+        <v>10</v>
+      </c>
+      <c r="L14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2.5</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>109</v>
+      </c>
+      <c r="D15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E15" t="s">
+        <v>68</v>
+      </c>
+      <c r="I15">
+        <v>10</v>
+      </c>
+      <c r="L15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>112</v>
+      </c>
+      <c r="D16" t="s">
+        <v>113</v>
+      </c>
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16">
+        <v>10</v>
+      </c>
+      <c r="L16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1.4</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" t="s">
+        <v>115</v>
+      </c>
+      <c r="E17" t="s">
+        <v>11</v>
+      </c>
+      <c r="I17">
+        <v>5</v>
+      </c>
+      <c r="L17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>6.1</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>114</v>
+      </c>
+      <c r="D18" t="s">
+        <v>118</v>
+      </c>
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+      <c r="I18">
+        <v>10</v>
+      </c>
+      <c r="L18" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2634,57 +2865,57 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.77734375" customWidth="1"/>
-    <col min="9" max="9" width="13.44140625" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:16" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="7"/>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="16" t="s">
+      <c r="D3" s="18"/>
+      <c r="E3" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16" t="s">
+      <c r="F3" s="19"/>
+      <c r="G3" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="J3" s="17" t="s">
+      <c r="J3" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>85</v>
       </c>
@@ -2703,9 +2934,9 @@
       <c r="F4" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="G4" s="16"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="G4" s="19"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>0</v>
       </c>
@@ -2729,7 +2960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>90</v>
       </c>
@@ -2757,11 +2988,11 @@
       <c r="H6" t="s">
         <v>99</v>
       </c>
-      <c r="I6" s="20" t="s">
+      <c r="I6" s="15" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>91</v>
       </c>
@@ -2786,9 +3017,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I7" s="18"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I7" s="13"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>93</v>
       </c>
@@ -2813,11 +3044,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I8" s="18" t="s">
+      <c r="I8" s="13" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>94</v>
       </c>
@@ -2842,9 +3073,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I9" s="18"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I9" s="13"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>92</v>
       </c>
@@ -2871,7 +3102,7 @@
       </c>
       <c r="J10" s="12"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>95</v>
       </c>
@@ -2896,10 +3127,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I11" s="19"/>
+      <c r="I11" s="14"/>
       <c r="J11" s="12"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>96</v>
       </c>
@@ -2924,12 +3155,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I12" s="19" t="s">
+      <c r="I12" s="14" t="s">
         <v>103</v>
       </c>
       <c r="J12" s="12"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>97</v>
       </c>
@@ -2954,10 +3185,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I13" s="19"/>
+      <c r="I13" s="14"/>
       <c r="J13" s="12"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>98</v>
       </c>
@@ -2985,13 +3216,13 @@
       <c r="H14" t="s">
         <v>100</v>
       </c>
-      <c r="I14" s="19"/>
+      <c r="I14" s="14"/>
       <c r="J14" s="12"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed the following bugs: Overview does now reload if a medicament is changed or added The dropdowns on the edit view now save and load if there is a value set delete works correct.
</commit_message>
<xml_diff>
--- a/Documents/Task 10/scrum_v02.xlsx
+++ b/Documents/Task 10/scrum_v02.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Turna\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="390" yWindow="120" windowWidth="16485" windowHeight="7815" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2448" windowWidth="16788" windowHeight="4608" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
@@ -18,7 +13,8 @@
     <sheet name="Sprint Work Time" sheetId="6" r:id="rId4"/>
     <sheet name="BurndownChart" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
+  <oleSize ref="A1:H13"/>
 </workbook>
 </file>
 
@@ -410,7 +406,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -699,9 +695,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="de-CH"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -793,7 +789,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-0578-4E58-90C1-91993B39FDE3}"/>
             </c:ext>
@@ -808,8 +804,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="239214040"/>
-        <c:axId val="239214432"/>
+        <c:axId val="109001344"/>
+        <c:axId val="109011712"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -880,7 +876,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-0578-4E58-90C1-91993B39FDE3}"/>
             </c:ext>
@@ -950,7 +946,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-0578-4E58-90C1-91993B39FDE3}"/>
             </c:ext>
@@ -966,11 +962,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="239214040"/>
-        <c:axId val="239214432"/>
+        <c:axId val="109001344"/>
+        <c:axId val="109011712"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="239214040"/>
+        <c:axId val="109001344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -999,6 +995,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1007,23 +1004,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx2"/>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1059,7 +1039,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239214432"/>
+        <c:crossAx val="109011712"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1069,7 +1049,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="239214432"/>
+        <c:axId val="109011712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1113,6 +1093,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1121,23 +1102,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx2"/>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1167,7 +1131,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239214040"/>
+        <c:crossAx val="109001344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1181,6 +1145,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1806,9 +1771,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1846,9 +1811,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1883,7 +1848,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1918,7 +1883,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2098,13 +2063,13 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="3" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -2112,7 +2077,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -2120,7 +2085,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -2128,7 +2093,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -2136,7 +2101,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -2144,7 +2109,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -2152,7 +2117,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -2169,23 +2134,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" customWidth="1"/>
-    <col min="2" max="2" width="33.5703125" customWidth="1"/>
-    <col min="3" max="3" width="38.42578125" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="33.5546875" customWidth="1"/>
+    <col min="3" max="3" width="38.44140625" customWidth="1"/>
+    <col min="4" max="4" width="9.44140625" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" customWidth="1"/>
+    <col min="6" max="6" width="19.5546875" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2211,7 +2176,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2228,7 +2193,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2246,7 +2211,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2263,7 +2228,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2280,7 +2245,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2297,7 +2262,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2314,7 +2279,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2331,7 +2296,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2348,7 +2313,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2365,7 +2330,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2413,24 +2378,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" customWidth="1"/>
-    <col min="4" max="4" width="85.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" customWidth="1"/>
-    <col min="11" max="11" width="7.28515625" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" customWidth="1"/>
+    <col min="3" max="3" width="26.88671875" customWidth="1"/>
+    <col min="4" max="4" width="85.44140625" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" customWidth="1"/>
+    <col min="9" max="9" width="7.88671875" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" customWidth="1"/>
+    <col min="11" max="11" width="7.33203125" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -2471,7 +2436,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1.1000000000000001</v>
       </c>
@@ -2503,7 +2468,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1.2</v>
       </c>
@@ -2535,7 +2500,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1.3</v>
       </c>
@@ -2567,7 +2532,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2.1</v>
       </c>
@@ -2599,7 +2564,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2.2000000000000002</v>
       </c>
@@ -2631,7 +2596,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2.2999999999999998</v>
       </c>
@@ -2663,7 +2628,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2.4</v>
       </c>
@@ -2727,7 +2692,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3.2</v>
       </c>
@@ -2759,7 +2724,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4.0999999999999996</v>
       </c>
@@ -2791,7 +2756,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1.4</v>
       </c>
@@ -2823,7 +2788,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>118</v>
       </c>
@@ -2856,7 +2821,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>115</v>
       </c>
@@ -2889,7 +2854,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
         <v>114</v>
       </c>
@@ -2922,7 +2887,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="22">
         <v>6.1</v>
       </c>
@@ -2955,7 +2920,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="22">
         <v>6.2</v>
       </c>
@@ -2988,7 +2953,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="30">
         <v>7.1</v>
       </c>
@@ -3019,7 +2984,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="30">
         <v>7.2</v>
       </c>
@@ -3060,13 +3025,13 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="27.85546875" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="27.88671875" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -3107,7 +3072,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>118</v>
       </c>
@@ -3132,7 +3097,7 @@
       <c r="K2" s="19"/>
       <c r="L2" s="19"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>115</v>
       </c>
@@ -3157,7 +3122,7 @@
       <c r="K3" s="19"/>
       <c r="L3" s="19"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>114</v>
       </c>
@@ -3182,7 +3147,7 @@
       <c r="K4" s="19"/>
       <c r="L4" s="19"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="19">
         <v>6.1</v>
       </c>
@@ -3207,7 +3172,7 @@
       <c r="K5" s="19"/>
       <c r="L5" s="19"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="19">
         <v>6.2</v>
       </c>
@@ -3232,7 +3197,7 @@
       <c r="K6" s="19"/>
       <c r="L6" s="19"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="27">
         <v>7.1</v>
       </c>
@@ -3257,7 +3222,7 @@
       <c r="K7" s="27"/>
       <c r="L7" s="27"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="27">
         <v>7.2</v>
       </c>
@@ -3296,11 +3261,11 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" customWidth="1"/>
+    <col min="9" max="9" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="31.5" x14ac:dyDescent="0.25">
@@ -3318,7 +3283,7 @@
       <c r="J1" s="32"/>
       <c r="K1" s="32"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
       <c r="B3" s="7"/>
       <c r="C3" s="33" t="s">
@@ -3342,7 +3307,7 @@
       <c r="O3" s="35"/>
       <c r="P3" s="35"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>85</v>
       </c>
@@ -3363,7 +3328,7 @@
       </c>
       <c r="G4" s="34"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>0</v>
       </c>
@@ -3387,7 +3352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>90</v>
       </c>
@@ -3419,7 +3384,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>91</v>
       </c>
@@ -3446,7 +3411,7 @@
       </c>
       <c r="I7" s="13"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>93</v>
       </c>
@@ -3475,7 +3440,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>94</v>
       </c>
@@ -3502,7 +3467,7 @@
       </c>
       <c r="I9" s="13"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>92</v>
       </c>
@@ -3529,7 +3494,7 @@
       </c>
       <c r="J10" s="12"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>95</v>
       </c>
@@ -3557,7 +3522,7 @@
       <c r="I11" s="14"/>
       <c r="J11" s="12"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>96</v>
       </c>
@@ -3587,7 +3552,7 @@
       </c>
       <c r="J12" s="12"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>97</v>
       </c>
@@ -3615,7 +3580,7 @@
       <c r="I13" s="14"/>
       <c r="J13" s="12"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>98</v>
       </c>
@@ -3646,10 +3611,10 @@
       <c r="I14" s="14"/>
       <c r="J14" s="12"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="10"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="11"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created first test for validation (methodOfApplication)
</commit_message>
<xml_diff>
--- a/Documents/Task 10/scrum_v02.xlsx
+++ b/Documents/Task 10/scrum_v02.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quantumli\workspace\ch.bfh.btx8081.w2015.schwarz\Documents\Task 10\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2448" windowWidth="16788" windowHeight="4608" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="16785" windowHeight="4605" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
@@ -13,8 +18,7 @@
     <sheet name="Sprint Work Time" sheetId="6" r:id="rId4"/>
     <sheet name="BurndownChart" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621"/>
-  <oleSize ref="A1:H13"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -406,7 +410,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -695,9 +699,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-CH"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -789,7 +793,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-0578-4E58-90C1-91993B39FDE3}"/>
             </c:ext>
@@ -876,7 +880,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-0578-4E58-90C1-91993B39FDE3}"/>
             </c:ext>
@@ -946,7 +950,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-0578-4E58-90C1-91993B39FDE3}"/>
             </c:ext>
@@ -995,7 +999,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1004,6 +1007,23 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1093,7 +1113,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1102,6 +1121,23 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1145,7 +1181,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1771,9 +1806,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1811,9 +1846,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1848,7 +1883,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1883,7 +1918,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2063,13 +2098,13 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="3" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -2077,7 +2112,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -2085,7 +2120,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -2093,7 +2128,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -2101,7 +2136,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -2109,7 +2144,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -2117,7 +2152,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -2134,23 +2169,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" customWidth="1"/>
-    <col min="2" max="2" width="33.5546875" customWidth="1"/>
-    <col min="3" max="3" width="38.44140625" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" customWidth="1"/>
-    <col min="6" max="6" width="19.5546875" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" customWidth="1"/>
-    <col min="8" max="8" width="14.44140625" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="33.5703125" customWidth="1"/>
+    <col min="3" max="3" width="38.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2176,7 +2211,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2193,7 +2228,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2211,7 +2246,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2228,7 +2263,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2245,7 +2280,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2262,7 +2297,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2279,7 +2314,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2296,7 +2331,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2313,7 +2348,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2330,7 +2365,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2378,24 +2413,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" customWidth="1"/>
-    <col min="2" max="2" width="6.33203125" customWidth="1"/>
-    <col min="3" max="3" width="26.88671875" customWidth="1"/>
-    <col min="4" max="4" width="85.44140625" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" customWidth="1"/>
-    <col min="9" max="9" width="7.88671875" customWidth="1"/>
-    <col min="10" max="10" width="9.109375" customWidth="1"/>
-    <col min="11" max="11" width="7.33203125" customWidth="1"/>
-    <col min="12" max="12" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" customWidth="1"/>
+    <col min="4" max="4" width="85.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" customWidth="1"/>
+    <col min="11" max="11" width="7.28515625" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -2436,7 +2471,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1.1000000000000001</v>
       </c>
@@ -2468,7 +2503,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1.2</v>
       </c>
@@ -2500,7 +2535,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1.3</v>
       </c>
@@ -2532,7 +2567,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2.1</v>
       </c>
@@ -2564,7 +2599,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2.2000000000000002</v>
       </c>
@@ -2596,7 +2631,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2.2999999999999998</v>
       </c>
@@ -2628,7 +2663,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2.4</v>
       </c>
@@ -2692,7 +2727,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3.2</v>
       </c>
@@ -2724,7 +2759,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4.0999999999999996</v>
       </c>
@@ -2753,10 +2788,10 @@
         <v>11</v>
       </c>
       <c r="L11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1.4</v>
       </c>
@@ -2788,7 +2823,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>118</v>
       </c>
@@ -2821,7 +2856,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>115</v>
       </c>
@@ -2854,7 +2889,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
         <v>114</v>
       </c>
@@ -2887,7 +2922,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="22">
         <v>6.1</v>
       </c>
@@ -2920,7 +2955,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="22">
         <v>6.2</v>
       </c>
@@ -2953,7 +2988,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="30">
         <v>7.1</v>
       </c>
@@ -2984,7 +3019,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="30">
         <v>7.2</v>
       </c>
@@ -3028,10 +3063,10 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="27.88671875" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -3072,7 +3107,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>118</v>
       </c>
@@ -3097,7 +3132,7 @@
       <c r="K2" s="19"/>
       <c r="L2" s="19"/>
     </row>
-    <row r="3" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>115</v>
       </c>
@@ -3122,7 +3157,7 @@
       <c r="K3" s="19"/>
       <c r="L3" s="19"/>
     </row>
-    <row r="4" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>114</v>
       </c>
@@ -3147,7 +3182,7 @@
       <c r="K4" s="19"/>
       <c r="L4" s="19"/>
     </row>
-    <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="19">
         <v>6.1</v>
       </c>
@@ -3172,7 +3207,7 @@
       <c r="K5" s="19"/>
       <c r="L5" s="19"/>
     </row>
-    <row r="6" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="19">
         <v>6.2</v>
       </c>
@@ -3197,7 +3232,7 @@
       <c r="K6" s="19"/>
       <c r="L6" s="19"/>
     </row>
-    <row r="7" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="27">
         <v>7.1</v>
       </c>
@@ -3222,7 +3257,7 @@
       <c r="K7" s="27"/>
       <c r="L7" s="27"/>
     </row>
-    <row r="8" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="27">
         <v>7.2</v>
       </c>
@@ -3261,11 +3296,11 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" customWidth="1"/>
-    <col min="9" max="9" width="13.44140625" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="31.5" x14ac:dyDescent="0.25">
@@ -3283,7 +3318,7 @@
       <c r="J1" s="32"/>
       <c r="K1" s="32"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="7"/>
       <c r="C3" s="33" t="s">
@@ -3307,7 +3342,7 @@
       <c r="O3" s="35"/>
       <c r="P3" s="35"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>85</v>
       </c>
@@ -3328,7 +3363,7 @@
       </c>
       <c r="G4" s="34"/>
     </row>
-    <row r="5" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>0</v>
       </c>
@@ -3352,7 +3387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>90</v>
       </c>
@@ -3384,7 +3419,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>91</v>
       </c>
@@ -3411,7 +3446,7 @@
       </c>
       <c r="I7" s="13"/>
     </row>
-    <row r="8" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>93</v>
       </c>
@@ -3440,7 +3475,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>94</v>
       </c>
@@ -3467,7 +3502,7 @@
       </c>
       <c r="I9" s="13"/>
     </row>
-    <row r="10" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>92</v>
       </c>
@@ -3494,7 +3529,7 @@
       </c>
       <c r="J10" s="12"/>
     </row>
-    <row r="11" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>95</v>
       </c>
@@ -3522,7 +3557,7 @@
       <c r="I11" s="14"/>
       <c r="J11" s="12"/>
     </row>
-    <row r="12" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>96</v>
       </c>
@@ -3552,7 +3587,7 @@
       </c>
       <c r="J12" s="12"/>
     </row>
-    <row r="13" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>97</v>
       </c>
@@ -3580,7 +3615,7 @@
       <c r="I13" s="14"/>
       <c r="J13" s="12"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>98</v>
       </c>
@@ -3611,10 +3646,10 @@
       <c r="I14" s="14"/>
       <c r="J14" s="12"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
     </row>
   </sheetData>

</xml_diff>